<commit_message>
Big update on code data handling
</commit_message>
<xml_diff>
--- a/aSYN.subset1.xlsx
+++ b/aSYN.subset1.xlsx
@@ -25,13 +25,13 @@
     <t xml:space="preserve">SSN</t>
   </si>
   <si>
-    <t xml:space="preserve">H</t>
+    <t xml:space="preserve">HN</t>
   </si>
   <si>
     <t xml:space="preserve">N</t>
   </si>
   <si>
-    <t xml:space="preserve">C</t>
+    <t xml:space="preserve">CO</t>
   </si>
   <si>
     <t xml:space="preserve">CA</t>
@@ -257,7 +257,7 @@
   <dimension ref="A1:AMJ105"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F:F"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>